<commit_message>
second task: gaussian regression
</commit_message>
<xml_diff>
--- a/P2/Gibbs energy inference.xlsx
+++ b/P2/Gibbs energy inference.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiaoyanyin/Desktop/ML_summer school/2019CAMMP/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" tabRatio="500"/>
+    <workbookView windowWidth="16020" windowHeight="7785" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,49 +14,29 @@
     <definedName name="dataset_B_2" localSheetId="0">Sheet1!$K$14:$O$19</definedName>
     <definedName name="Fe_Cr_C_Data" localSheetId="0">Sheet1!$A$2:$D$98</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="dataset_A11" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/xiaoyanyin/Desktop/ML_summer school/2019CAMMP/Fe_Cr_C_Gibbs/dataset_A.csv" thousands="'" comma="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="1" name="dataset_A11" type="6" background="1" refreshedVersion="2" saveData="1">
+    <textPr sourceFile="/Users/xiaoyanyin/Desktop/ML_summer school/2019CAMMP/Fe_Cr_C_Gibbs/dataset_A.csv" thousands="'" comma="1">
+      <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="dataset_B11" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/xiaoyanyin/Desktop/ML_summer school/2019CAMMP/Fe_Cr_C_Gibbs/dataset_B.csv" thousands="'" comma="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="2" name="dataset_B11" type="6" background="1" refreshedVersion="2" saveData="1">
+    <textPr sourceFile="/Users/xiaoyanyin/Desktop/ML_summer school/2019CAMMP/Fe_Cr_C_Gibbs/dataset_B.csv" thousands="'" comma="1">
+      <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="Fe_Cr_C_Data" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" sourceFile="/Users/xiaoyanyin/Desktop/ML_summer school/2019CAMMP/Fe_Cr_C_Gibbs/Fe_Cr_C_Data.csv" thousands="'" comma="1">
-      <textFields count="5">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="3" name="Fe_Cr_C_Data" type="6" background="1" refreshedVersion="2" saveData="1">
+    <textPr sourceFile="/Users/xiaoyanyin/Desktop/ML_summer school/2019CAMMP/Fe_Cr_C_Gibbs/Fe_Cr_C_Data.csv" thousands="'" comma="1">
+      <textFields>
         <textField/>
       </textFields>
     </textPr>
@@ -72,6 +47,18 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="18">
   <si>
+    <t>Fe-C system</t>
+  </si>
+  <si>
+    <t>Fe-Cr system</t>
+  </si>
+  <si>
+    <t>Fe-C-Cr system</t>
+  </si>
+  <si>
+    <t>Wt-% C</t>
+  </si>
+  <si>
     <t>T/K</t>
   </si>
   <si>
@@ -81,13 +68,25 @@
     <t>phase</t>
   </si>
   <si>
+    <t>Wt-% Cr</t>
+  </si>
+  <si>
     <t>gamma</t>
   </si>
   <si>
-    <t>alpha</t>
+    <t>gamma+M7C3</t>
+  </si>
+  <si>
+    <t>gamma+cementite</t>
+  </si>
+  <si>
+    <t>M7C3+graphite</t>
   </si>
   <si>
     <t>alpha+gamma</t>
+  </si>
+  <si>
+    <t>alpha</t>
   </si>
   <si>
     <t>gamma+graphite</t>
@@ -101,74 +100,396 @@
   <si>
     <t>gamma+graphite96</t>
   </si>
-  <si>
-    <t>Wt-% Cr</t>
-  </si>
-  <si>
-    <t>Wt-% C</t>
-  </si>
-  <si>
-    <t>gamma+M7C3</t>
-  </si>
-  <si>
-    <t>gamma+cementite</t>
-  </si>
-  <si>
-    <t>M7C3+graphite</t>
-  </si>
-  <si>
-    <t>Fe-C system</t>
-  </si>
-  <si>
-    <t>Fe-Cr system</t>
-  </si>
-  <si>
-    <t>Fe-C-Cr system</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFC00000"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF7030A0"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="9" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="DengXian"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="DengXian"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -176,9 +497,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -192,10 +755,57 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -260,7 +870,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -295,7 +905,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -469,100 +1079,95 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.16666666666667" customWidth="1"/>
+    <col min="2" max="2" width="5.16666666666667" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="21.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6666666666667" customWidth="1"/>
+    <col min="9" max="9" width="13.6666666666667" customWidth="1"/>
+    <col min="10" max="10" width="21.1666666666667" customWidth="1"/>
     <col min="14" max="14" width="26.5" customWidth="1"/>
     <col min="15" max="15" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="F1" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="K1" s="3" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3">
-        <v>6.0000000000000001E-3</v>
+        <v>0.006</v>
       </c>
       <c r="B3">
         <v>1273</v>
@@ -571,7 +1176,7 @@
         <v>-61816.4</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>0.01</v>
@@ -583,13 +1188,13 @@
         <v>-62737.2</v>
       </c>
       <c r="I3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K3">
         <v>0.09</v>
       </c>
       <c r="L3">
-        <v>6.0000000000000001E-3</v>
+        <v>0.006</v>
       </c>
       <c r="M3">
         <v>1273</v>
@@ -598,12 +1203,12 @@
         <v>-63765.1</v>
       </c>
       <c r="O3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="B4">
         <v>1300</v>
@@ -612,7 +1217,7 @@
         <v>-64074.8</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F4">
         <v>0.02</v>
@@ -624,27 +1229,27 @@
         <v>-63027.7</v>
       </c>
       <c r="I4" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K4">
         <v>0.08</v>
       </c>
       <c r="L4">
-        <v>4.0000000000000001E-3</v>
+        <v>0.004</v>
       </c>
       <c r="M4">
         <v>1373</v>
       </c>
       <c r="N4">
-        <v>-71999.100000000006</v>
+        <v>-71999.1</v>
       </c>
       <c r="O4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
-        <v>4.0000000000000001E-3</v>
+        <v>0.004</v>
       </c>
       <c r="B5">
         <v>1300</v>
@@ -653,7 +1258,7 @@
         <v>-64189.9</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>0.02</v>
@@ -665,36 +1270,36 @@
         <v>-65176.7</v>
       </c>
       <c r="I5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K5">
         <v>0.05</v>
       </c>
       <c r="L5">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="M5">
         <v>1473</v>
       </c>
       <c r="N5">
-        <v>-80141.600000000006</v>
+        <v>-80141.6</v>
       </c>
       <c r="O5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
-        <v>3.5000000000000001E-3</v>
+        <v>0.0035</v>
       </c>
       <c r="B6">
         <v>1473</v>
       </c>
       <c r="C6">
-        <v>-78360.600000000006</v>
+        <v>-78360.6</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>0.03</v>
@@ -706,13 +1311,13 @@
         <v>-67019.8</v>
       </c>
       <c r="I6" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K6">
         <v>0.1</v>
       </c>
       <c r="L6">
-        <v>6.0000000000000001E-3</v>
+        <v>0.006</v>
       </c>
       <c r="M6">
         <v>1473</v>
@@ -721,12 +1326,12 @@
         <v>-80463.5</v>
       </c>
       <c r="O6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="B7">
         <v>1350</v>
@@ -735,7 +1340,7 @@
         <v>-68375</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F7">
         <v>0.09</v>
@@ -744,16 +1349,16 @@
         <v>1320</v>
       </c>
       <c r="H7">
-        <v>-67828.899999999994</v>
+        <v>-67828.9</v>
       </c>
       <c r="I7" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K7">
         <v>0.1</v>
       </c>
       <c r="L7">
-        <v>5.5999999999999999E-3</v>
+        <v>0.0056</v>
       </c>
       <c r="M7">
         <v>1273</v>
@@ -762,21 +1367,21 @@
         <v>-63891.7</v>
       </c>
       <c r="O7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8">
-        <v>1.5E-3</v>
+        <v>0.0015</v>
       </c>
       <c r="B8">
         <v>1320</v>
       </c>
       <c r="C8">
-        <v>-65999.100000000006</v>
+        <v>-65999.1</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <v>0.05</v>
@@ -788,7 +1393,7 @@
         <v>-74956</v>
       </c>
       <c r="I8" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K8">
         <v>0.02</v>
@@ -803,12 +1408,12 @@
         <v>-60397.1</v>
       </c>
       <c r="O8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="B9">
         <v>1273</v>
@@ -817,10 +1422,10 @@
         <v>-62299.6</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>4.2999999999999997E-2</v>
+        <v>0.043</v>
       </c>
       <c r="G9">
         <v>1390</v>
@@ -829,7 +1434,7 @@
         <v>-73003</v>
       </c>
       <c r="I9" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K9">
         <v>0.18</v>
@@ -844,24 +1449,24 @@
         <v>-63514.2</v>
       </c>
       <c r="O9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="B10">
         <v>1473</v>
       </c>
       <c r="C10">
-        <v>-78540.100000000006</v>
+        <v>-78540.1</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F10">
-        <v>3.7999999999999999E-2</v>
+        <v>0.038</v>
       </c>
       <c r="G10">
         <v>1295</v>
@@ -870,13 +1475,13 @@
         <v>-65167.8</v>
       </c>
       <c r="I10" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K10">
         <v>0.03</v>
       </c>
       <c r="L10">
-        <v>3.0000000000000001E-3</v>
+        <v>0.003</v>
       </c>
       <c r="M10">
         <v>1350</v>
@@ -885,39 +1490,39 @@
         <v>-69364</v>
       </c>
       <c r="O10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11">
-        <v>5.1999999999999998E-3</v>
+        <v>0.0052</v>
       </c>
       <c r="B11">
         <v>1380</v>
       </c>
       <c r="C11">
-        <v>-70482.899999999994</v>
+        <v>-70482.9</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F11">
-        <v>7.1999999999999995E-2</v>
+        <v>0.072</v>
       </c>
       <c r="G11">
         <v>1300</v>
       </c>
       <c r="H11">
-        <v>-66042.899999999994</v>
+        <v>-66042.9</v>
       </c>
       <c r="I11" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K11">
         <v>0.12</v>
       </c>
       <c r="L11">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M11">
         <v>1100</v>
@@ -926,21 +1531,21 @@
         <v>-50434.6</v>
       </c>
       <c r="O11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12">
-        <v>4.4999999999999997E-3</v>
+        <v>0.0045</v>
       </c>
       <c r="B12">
         <v>1410</v>
       </c>
       <c r="C12">
-        <v>-73021.899999999994</v>
+        <v>-73021.9</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F12">
         <v>0.08</v>
@@ -952,13 +1557,13 @@
         <v>-78565.2</v>
       </c>
       <c r="I12" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K12">
         <v>0.2</v>
       </c>
       <c r="L12">
-        <v>1.6E-2</v>
+        <v>0.016</v>
       </c>
       <c r="M12">
         <v>1500</v>
@@ -967,12 +1572,12 @@
         <v>-82362</v>
       </c>
       <c r="O12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13">
-        <v>5.0000000000000001E-4</v>
+        <v>0.0005</v>
       </c>
       <c r="B13">
         <v>1280</v>
@@ -981,25 +1586,25 @@
         <v>-62861</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>6.3E-2</v>
+        <v>0.063</v>
       </c>
       <c r="G13">
         <v>1473</v>
       </c>
       <c r="H13">
-        <v>-80307.100000000006</v>
+        <v>-80307.1</v>
       </c>
       <c r="I13" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K13">
         <v>0.19</v>
       </c>
       <c r="L13">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="M13">
         <v>1500</v>
@@ -1008,24 +1613,24 @@
         <v>-81651.3</v>
       </c>
       <c r="O13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
-        <v>6.9999999999999999E-4</v>
+        <v>0.0007</v>
       </c>
       <c r="B14">
         <v>1473</v>
       </c>
       <c r="C14">
-        <v>-78545.399999999994</v>
+        <v>-78545.4</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F14">
-        <v>5.8000000000000003E-2</v>
+        <v>0.058</v>
       </c>
       <c r="G14">
         <v>1460</v>
@@ -1034,12 +1639,12 @@
         <v>-79126</v>
       </c>
       <c r="I14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15">
-        <v>5.7000000000000002E-3</v>
+        <v>0.0057</v>
       </c>
       <c r="B15">
         <v>1450</v>
@@ -1048,10 +1653,10 @@
         <v>-76182</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F15">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="G15">
         <v>1473</v>
@@ -1060,10 +1665,10 @@
         <v>-79230</v>
       </c>
       <c r="I15" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K15">
-        <v>0.28000000000000003</v>
+        <v>0.28</v>
       </c>
       <c r="L15">
         <v>0.03</v>
@@ -1075,12 +1680,12 @@
         <v>-73574.2</v>
       </c>
       <c r="O15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16">
-        <v>1.2999999999999999E-3</v>
+        <v>0.0013</v>
       </c>
       <c r="B16">
         <v>1473</v>
@@ -1089,10 +1694,10 @@
         <v>-78529.5</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F16">
-        <v>2.3E-2</v>
+        <v>0.023</v>
       </c>
       <c r="G16">
         <v>1380</v>
@@ -1101,7 +1706,7 @@
         <v>-71736.2</v>
       </c>
       <c r="I16" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K16">
         <v>0.3</v>
@@ -1116,12 +1721,12 @@
         <v>-58107.1</v>
       </c>
       <c r="O16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17">
-        <v>2.9999999999999997E-4</v>
+        <v>0.0003</v>
       </c>
       <c r="B17">
         <v>1300</v>
@@ -1130,10 +1735,10 @@
         <v>-64438.7</v>
       </c>
       <c r="D17" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F17">
-        <v>8.5999999999999993E-2</v>
+        <v>0.086</v>
       </c>
       <c r="G17">
         <v>1280</v>
@@ -1142,7 +1747,7 @@
         <v>-64554.8</v>
       </c>
       <c r="I17" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K17">
         <v>0.5</v>
@@ -1154,39 +1759,39 @@
         <v>1500</v>
       </c>
       <c r="N17">
-        <v>-75724.600000000006</v>
+        <v>-75724.6</v>
       </c>
       <c r="O17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18">
-        <v>3.8E-3</v>
+        <v>0.0038</v>
       </c>
       <c r="B18">
         <v>1290</v>
       </c>
       <c r="C18">
-        <v>-63419.199999999997</v>
+        <v>-63419.2</v>
       </c>
       <c r="D18" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F18">
-        <v>9.7000000000000003E-2</v>
+        <v>0.097</v>
       </c>
       <c r="G18">
         <v>1310</v>
       </c>
       <c r="H18">
-        <v>-67062.899999999994</v>
+        <v>-67062.9</v>
       </c>
       <c r="I18" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K18">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="L18">
         <v>0.06</v>
@@ -1195,24 +1800,24 @@
         <v>1373</v>
       </c>
       <c r="N18">
-        <v>-68650.899999999994</v>
+        <v>-68650.9</v>
       </c>
       <c r="O18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19">
-        <v>2.2000000000000001E-3</v>
+        <v>0.0022</v>
       </c>
       <c r="B19">
         <v>1410</v>
       </c>
       <c r="C19">
-        <v>-73246.899999999994</v>
+        <v>-73246.9</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F19">
         <v>0.1</v>
@@ -1224,13 +1829,13 @@
         <v>-64085.5</v>
       </c>
       <c r="I19" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K19">
         <v>0.255</v>
       </c>
       <c r="L19">
-        <v>2.1999999999999999E-2</v>
+        <v>0.022</v>
       </c>
       <c r="M19">
         <v>1400</v>
@@ -1239,12 +1844,12 @@
         <v>-73974.7</v>
       </c>
       <c r="O19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
-        <v>1.6999999999999999E-3</v>
+        <v>0.0017</v>
       </c>
       <c r="B20">
         <v>1350</v>
@@ -1253,7 +1858,7 @@
         <v>-68395</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F20">
         <v>0.04</v>
@@ -1262,15 +1867,15 @@
         <v>1350</v>
       </c>
       <c r="H20">
-        <v>-69657.100000000006</v>
+        <v>-69657.1</v>
       </c>
       <c r="I20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
-        <v>4.7999999999999996E-3</v>
+        <v>0.0048</v>
       </c>
       <c r="B21">
         <v>1280</v>
@@ -1279,10 +1884,10 @@
         <v>-62517</v>
       </c>
       <c r="D21" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F21">
-        <v>9.0999999999999998E-2</v>
+        <v>0.091</v>
       </c>
       <c r="G21">
         <v>1373</v>
@@ -1291,12 +1896,12 @@
         <v>-72201.5</v>
       </c>
       <c r="I21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
-        <v>6.0000000000000001E-3</v>
+        <v>0.006</v>
       </c>
       <c r="B22">
         <v>1473</v>
@@ -1305,7 +1910,7 @@
         <v>-78062.2</v>
       </c>
       <c r="D22" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F22">
         <v>0.08</v>
@@ -1317,21 +1922,21 @@
         <v>-63942.9</v>
       </c>
       <c r="I22" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="B23">
         <v>1073</v>
       </c>
       <c r="C23">
-        <v>-47205.599999999999</v>
+        <v>-47205.6</v>
       </c>
       <c r="D23" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F23">
         <v>0.11</v>
@@ -1343,12 +1948,12 @@
         <v>-36638.9</v>
       </c>
       <c r="I23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="B24">
         <v>1073</v>
@@ -1357,7 +1962,7 @@
         <v>-47101.4</v>
       </c>
       <c r="D24" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F24">
         <v>0.11</v>
@@ -1369,12 +1974,12 @@
         <v>-74588.7</v>
       </c>
       <c r="I24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="B25">
         <v>1073</v>
@@ -1383,7 +1988,7 @@
         <v>-46778.3</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F25">
         <v>0.11</v>
@@ -1392,13 +1997,13 @@
         <v>1460</v>
       </c>
       <c r="H25">
-        <v>-79689.899999999994</v>
+        <v>-79689.9</v>
       </c>
       <c r="I25" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>0.01</v>
       </c>
@@ -1409,7 +2014,7 @@
         <v>-46097</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F26">
         <v>0.11</v>
@@ -1421,12 +2026,12 @@
         <v>-98576.9</v>
       </c>
       <c r="I26" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="B27">
         <v>1170</v>
@@ -1435,7 +2040,7 @@
         <v>-52975.3</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F27">
         <v>0.12</v>
@@ -1444,24 +2049,24 @@
         <v>1273</v>
       </c>
       <c r="H27">
-        <v>-64177.599999999999</v>
+        <v>-64177.6</v>
       </c>
       <c r="I27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
-        <v>1.4E-2</v>
+        <v>0.014</v>
       </c>
       <c r="B28">
         <v>1200</v>
       </c>
       <c r="C28">
-        <v>-54922.400000000001</v>
+        <v>-54922.4</v>
       </c>
       <c r="D28" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F28">
         <v>0.1</v>
@@ -1473,10 +2078,10 @@
         <v>-78749.2</v>
       </c>
       <c r="I28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>0.02</v>
       </c>
@@ -1487,7 +2092,7 @@
         <v>-67380.2</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F29">
         <v>0.2</v>
@@ -1499,12 +2104,12 @@
         <v>-43402.6</v>
       </c>
       <c r="I29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
-        <v>1.7999999999999999E-2</v>
+        <v>0.018</v>
       </c>
       <c r="B30">
         <v>1373</v>
@@ -1513,7 +2118,7 @@
         <v>-67773.5</v>
       </c>
       <c r="D30" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F30">
         <v>0.2</v>
@@ -1525,21 +2130,21 @@
         <v>-70693</v>
       </c>
       <c r="I30" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="B31">
         <v>1373</v>
       </c>
       <c r="C31">
-        <v>-67576.399999999994</v>
+        <v>-67576.4</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F31">
         <v>0.2</v>
@@ -1551,12 +2156,12 @@
         <v>-101556</v>
       </c>
       <c r="I31" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
-        <v>1.7000000000000001E-2</v>
+        <v>0.017</v>
       </c>
       <c r="B32">
         <v>1273</v>
@@ -1565,7 +2170,7 @@
         <v>-60027.7</v>
       </c>
       <c r="D32" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F32">
         <v>0.25</v>
@@ -1577,12 +2182,12 @@
         <v>-58426.5</v>
       </c>
       <c r="I32" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
-        <v>1.7000000000000001E-2</v>
+        <v>0.017</v>
       </c>
       <c r="B33">
         <v>1330</v>
@@ -1591,7 +2196,7 @@
         <v>-64517.9</v>
       </c>
       <c r="D33" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F33">
         <v>0.25</v>
@@ -1600,15 +2205,15 @@
         <v>1473</v>
       </c>
       <c r="H33">
-        <v>-81120.100000000006</v>
+        <v>-81120.1</v>
       </c>
       <c r="I33" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
-        <v>1.7000000000000001E-2</v>
+        <v>0.017</v>
       </c>
       <c r="B34">
         <v>1400</v>
@@ -1617,7 +2222,7 @@
         <v>-70158.3</v>
       </c>
       <c r="D34" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F34">
         <v>0.25</v>
@@ -1629,21 +2234,21 @@
         <v>-92371</v>
       </c>
       <c r="I34" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
-        <v>8.9999999999999993E-3</v>
+        <v>0.009</v>
       </c>
       <c r="B35">
         <v>1000</v>
       </c>
       <c r="C35">
-        <v>-41078.400000000001</v>
+        <v>-41078.4</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F35">
         <v>0.15</v>
@@ -1655,12 +2260,12 @@
         <v>-64287.4</v>
       </c>
       <c r="I35" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
-        <v>8.9999999999999993E-3</v>
+        <v>0.009</v>
       </c>
       <c r="B36">
         <v>1050</v>
@@ -1669,7 +2274,7 @@
         <v>-44576.7</v>
       </c>
       <c r="D36" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F36">
         <v>0.17</v>
@@ -1678,15 +2283,15 @@
         <v>1400</v>
       </c>
       <c r="H36">
-        <v>-74866.100000000006</v>
+        <v>-74866.1</v>
       </c>
       <c r="I36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
-        <v>7.0000000000000001E-3</v>
+        <v>0.007</v>
       </c>
       <c r="B37">
         <v>1050</v>
@@ -1695,7 +2300,7 @@
         <v>-44854.5</v>
       </c>
       <c r="D37" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F37">
         <v>0.18</v>
@@ -1704,15 +2309,15 @@
         <v>1373</v>
       </c>
       <c r="H37">
-        <v>-72605.100000000006</v>
+        <v>-72605.1</v>
       </c>
       <c r="I37" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
-        <v>7.0000000000000001E-3</v>
+        <v>0.007</v>
       </c>
       <c r="B38">
         <v>1010</v>
@@ -1721,7 +2326,7 @@
         <v>-41998.1</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F38">
         <v>0.13</v>
@@ -1733,21 +2338,21 @@
         <v>-64217.3</v>
       </c>
       <c r="I38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="B39">
         <v>1010</v>
       </c>
       <c r="C39">
-        <v>-41865.800000000003</v>
+        <v>-41865.8</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F39">
         <v>0.13</v>
@@ -1759,12 +2364,12 @@
         <v>-72443.5</v>
       </c>
       <c r="I39" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="B40">
         <v>1050</v>
@@ -1773,10 +2378,10 @@
         <v>-44716.5</v>
       </c>
       <c r="D40" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="F40">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="G40">
         <v>1273</v>
@@ -1785,12 +2390,12 @@
         <v>-64255.7</v>
       </c>
       <c r="I40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="B41">
         <v>1230</v>
@@ -1799,7 +2404,7 @@
         <v>-58185.8</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F41">
         <v>0.123</v>
@@ -1808,24 +2413,24 @@
         <v>1300</v>
       </c>
       <c r="H41">
-        <v>-66378.899999999994</v>
+        <v>-66378.9</v>
       </c>
       <c r="I41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="B42">
         <v>1473</v>
       </c>
       <c r="C42">
-        <v>-77775.100000000006</v>
+        <v>-77775.1</v>
       </c>
       <c r="D42" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F42">
         <v>0.123</v>
@@ -1837,12 +2442,12 @@
         <v>-74673.2</v>
       </c>
       <c r="I42" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43">
-        <v>4.0000000000000001E-3</v>
+        <v>0.004</v>
       </c>
       <c r="B43">
         <v>1050</v>
@@ -1851,7 +2456,7 @@
         <v>-45226.3</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F43">
         <v>0.15</v>
@@ -1863,12 +2468,12 @@
         <v>-43444.4</v>
       </c>
       <c r="I43" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44">
-        <v>1.1999999999999999E-3</v>
+        <v>0.0012</v>
       </c>
       <c r="B44">
         <v>1100</v>
@@ -1877,7 +2482,7 @@
         <v>-49133</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F44">
         <v>0.15</v>
@@ -1886,15 +2491,15 @@
         <v>1390</v>
       </c>
       <c r="H44">
-        <v>-73961.399999999994</v>
+        <v>-73961.4</v>
       </c>
       <c r="I44" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
-        <v>1.2999999999999999E-3</v>
+        <v>0.0013</v>
       </c>
       <c r="B45">
         <v>1100</v>
@@ -1903,7 +2508,7 @@
         <v>-49124.4</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F45">
         <v>0.05</v>
@@ -1915,12 +2520,12 @@
         <v>-97621.6</v>
       </c>
       <c r="I45" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46">
-        <v>1.1999999999999999E-3</v>
+        <v>0.0012</v>
       </c>
       <c r="B46">
         <v>1573</v>
@@ -1929,10 +2534,10 @@
         <v>-87031.1</v>
       </c>
       <c r="D46" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>0.01</v>
       </c>
@@ -1943,12 +2548,12 @@
         <v>-85938.8</v>
       </c>
       <c r="D47" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="B48">
         <v>1300</v>
@@ -1957,12 +2562,12 @@
         <v>-62509.5</v>
       </c>
       <c r="D48" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="B49">
         <v>1273</v>
@@ -1971,12 +2576,12 @@
         <v>-60908.9</v>
       </c>
       <c r="D49" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50">
-        <v>1.2999999999999999E-2</v>
+        <v>0.013</v>
       </c>
       <c r="B50">
         <v>1373</v>
@@ -1985,26 +2590,26 @@
         <v>-68709.2</v>
       </c>
       <c r="D50" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51">
-        <v>1.4E-2</v>
+        <v>0.014</v>
       </c>
       <c r="B51">
         <v>1473</v>
       </c>
       <c r="C51">
-        <v>-76749.399999999994</v>
+        <v>-76749.4</v>
       </c>
       <c r="D51" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
       <c r="A52">
-        <v>1.6E-2</v>
+        <v>0.016</v>
       </c>
       <c r="B52">
         <v>1273</v>
@@ -2013,40 +2618,40 @@
         <v>-60206.1</v>
       </c>
       <c r="D52" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53">
-        <v>1.6E-2</v>
+        <v>0.016</v>
       </c>
       <c r="B53">
         <v>1380</v>
       </c>
       <c r="C53">
-        <v>-68725.600000000006</v>
+        <v>-68725.6</v>
       </c>
       <c r="D53" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
       <c r="A54">
-        <v>1.6E-2</v>
+        <v>0.016</v>
       </c>
       <c r="B54">
         <v>1473</v>
       </c>
       <c r="C54">
-        <v>-76367.399999999994</v>
+        <v>-76367.4</v>
       </c>
       <c r="D54" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
       <c r="A55">
-        <v>1.7500000000000002E-2</v>
+        <v>0.0175</v>
       </c>
       <c r="B55">
         <v>1300</v>
@@ -2055,7 +2660,7 @@
         <v>-62050.1</v>
       </c>
       <c r="D55" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2065,5 +2670,6 @@
     <mergeCell ref="K1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>